<commit_message>
modified plot routines, now including drainage new sample report files, including the last 2 wards of Ramani Huria 1.0
</commit_message>
<xml_diff>
--- a/sample_data/report_files/crossings_report.xlsx
+++ b/sample_data/report_files/crossings_report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Buguruni</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Manzese</t>
   </si>
   <si>
+    <t>Mburahati</t>
+  </si>
+  <si>
     <t>Mchikichini</t>
   </si>
   <si>
@@ -68,6 +71,9 @@
   </si>
   <si>
     <t>Temeke</t>
+  </si>
+  <si>
+    <t>Ubungo</t>
   </si>
   <si>
     <t>Vingunguti</t>
@@ -91,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,12 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -158,11 +161,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -241,7 +239,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -276,7 +273,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,18 +448,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -522,10 +516,16 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>76</v>
@@ -558,36 +558,42 @@
         <v>106</v>
       </c>
       <c r="L2">
+        <v>27</v>
+      </c>
+      <c r="M2">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>78</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>57</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>73</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>25</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>82</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>41</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>71</v>
       </c>
-      <c r="T2">
+      <c r="U2">
+        <v>96</v>
+      </c>
+      <c r="V2">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>268</v>
@@ -620,36 +626,42 @@
         <v>318</v>
       </c>
       <c r="L3">
+        <v>155</v>
+      </c>
+      <c r="M3">
         <v>136</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>88</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>120</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>68</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>241</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>158</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>270</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>48</v>
       </c>
-      <c r="T3">
+      <c r="U3">
+        <v>126</v>
+      </c>
+      <c r="V3">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -682,36 +694,42 @@
         <v>6</v>
       </c>
       <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>3</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>3</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>6</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>5</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>14</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>0</v>
       </c>
-      <c r="T4">
+      <c r="U4">
+        <v>15</v>
+      </c>
+      <c r="V4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>71</v>
@@ -744,35 +762,38 @@
         <v>99</v>
       </c>
       <c r="L5">
+        <v>22</v>
+      </c>
+      <c r="M5">
         <v>8</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>75</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>56</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>70</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>18</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>77</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>26</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>71</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="V5">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>